<commit_message>
Initial commit: Add baru
</commit_message>
<xml_diff>
--- a/Test Case.xlsx
+++ b/Test Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ed32f76869c4bcf9/Desktop/demoblaze-senior-qa-portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="492" documentId="13_ncr:1_{F77A294A-C378-421B-B5C6-AECAE87A1321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C4D9270-0261-4E09-B776-AB7972E53929}"/>
+  <xr:revisionPtr revIDLastSave="494" documentId="13_ncr:1_{F77A294A-C378-421B-B5C6-AECAE87A1321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAA0D0C0-6EF6-4097-840E-69C5F0AC3453}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{739BE312-AA31-4B31-A566-DB081319E3AB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="326">
   <si>
     <t xml:space="preserve">Pre-condition:  </t>
   </si>
@@ -1414,6 +1414,9 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
   </si>
 </sst>
 </file>
@@ -4300,7 +4303,7 @@
   <dimension ref="A1:P121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="L62" sqref="L62:M65"/>
+      <selection activeCell="P62" sqref="P62:P65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5639,7 +5642,7 @@
       </c>
       <c r="O62" s="51"/>
       <c r="P62" s="79" t="s">
-        <v>293</v>
+        <v>325</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>